<commit_message>
november sheet question updated
</commit_message>
<xml_diff>
--- a/november.xlsx
+++ b/november.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAVIJ PARIKH\Desktop\aditya verma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3DAD84-26CF-42FE-B33C-E16AEB44A7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9266E0-15FA-4821-AEA9-5EBC1A2D276A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>DATE</t>
   </si>
@@ -79,6 +79,39 @@
   </si>
   <si>
     <t>BINARY SEARCH</t>
+  </si>
+  <si>
+    <t>K Closest Pair to Origin</t>
+  </si>
+  <si>
+    <t>Two Sum</t>
+  </si>
+  <si>
+    <t>Find Maximum Ones</t>
+  </si>
+  <si>
+    <t>Minimum Number Games</t>
+  </si>
+  <si>
+    <t>LEETCODE</t>
+  </si>
+  <si>
+    <t>Connect Ropes To Minimize Cost</t>
+  </si>
+  <si>
+    <t>INTERVIEW BIT</t>
+  </si>
+  <si>
+    <t>Binary Search for Descended Sorted Array</t>
+  </si>
+  <si>
+    <t>First and Last Occurrence of element</t>
+  </si>
+  <si>
+    <t>Order Agnostic Search</t>
+  </si>
+  <si>
+    <t>GFG</t>
   </si>
 </sst>
 </file>
@@ -126,11 +159,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,16 +445,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.109375" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="43.77734375" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" customWidth="1"/>
   </cols>
@@ -565,6 +599,118 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45964</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>45965</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>45965</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45966</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45966</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45967</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45967</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45967</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
binary search questions added
</commit_message>
<xml_diff>
--- a/november.xlsx
+++ b/november.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAVIJ PARIKH\Desktop\aditya verma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9266E0-15FA-4821-AEA9-5EBC1A2D276A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2235A0-9AEA-41D8-BA65-0ABE916FA253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>DATE</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>GFG</t>
+  </si>
+  <si>
+    <t>Count of an element in array</t>
+  </si>
+  <si>
+    <t>Number of times sorted array is rotated</t>
   </si>
 </sst>
 </file>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,6 +717,34 @@
         <v>28</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45968</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45968</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>